<commit_message>
Allow the user prompt to be overridden (primarily so we know we're definitely using the game-specific module)
</commit_message>
<xml_diff>
--- a/house.xlsx
+++ b/house.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work-in-progress\kelston-coding\adventure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7B91EC9-CD2B-4237-BC6A-94F705397BDF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AA25765-0278-4D0E-9D42-17D981F6A5B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -561,7 +561,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="D15" sqref="D14:D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -689,7 +689,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04CBE6F7-8E16-4651-B353-26513C8E6461}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>